<commit_message>
Updated with new logic and adjustmets from Elevresor
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon27san\Documents\UiPath\Masterfil För Skolskjuts\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon27san\Documents\UiPath\Masterfil För Skolskjuts Elevresor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
   </si>
   <si>
     <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
@@ -218,12 +215,6 @@
     <t>LimitOfHowOldSubmissionDate</t>
   </si>
   <si>
-    <t>SignProtectedCitizenID</t>
-  </si>
-  <si>
-    <t>SignTFCitizenID</t>
-  </si>
-  <si>
     <t>LimitOfHowSoonDecisionIsValid</t>
   </si>
   <si>
@@ -294,6 +285,22 @@
   </si>
   <si>
     <t>Ärendet har inte längre än beviljad status</t>
+  </si>
+  <si>
+    <t>TempFilesPath</t>
+  </si>
+  <si>
+    <t>CaseMayNotBeValid</t>
+  </si>
+  <si>
+    <t>Kan ej avgöra</t>
+  </si>
+  <si>
+    <t>CaseHasProtectedId</t>
+  </si>
+  <si>
+    <t>Skyddat Personnummer
+Skyddat personnummer</t>
   </si>
 </sst>
 </file>
@@ -670,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -720,139 +727,153 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" t="s">
-        <v>82</v>
-      </c>
-    </row>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1831,6 +1852,7 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1843,7 +1865,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1896,18 +1918,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1916,112 +1938,112 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3003,10 +3025,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3025,7 +3047,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3055,139 +3077,134 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
@@ -4167,8 +4184,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First commit to prod
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -189,15 +189,6 @@
   </si>
   <si>
     <t>ControlFileNeededInformation</t>
-  </si>
-  <si>
-    <t>OeP_MessageNoLongerValid</t>
-  </si>
-  <si>
-    <t>OeP_StatusNoLongerValid</t>
-  </si>
-  <si>
-    <t>OeP_StatusNotApproved</t>
   </si>
   <si>
     <t>LatestRun</t>
@@ -727,7 +718,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -765,102 +756,102 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1927,7 +1918,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -3014,10 +3005,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3122,93 +3113,72 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>56</v>
+      <c r="A12" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>57</v>
+      <c r="A13" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>58</v>
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -4170,9 +4140,6 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: Some updates around protected ids etc
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -289,6 +289,15 @@
   </si>
   <si>
     <t>FilterNOTApprovedCases</t>
+  </si>
+  <si>
+    <t>EmailAdress_To_Verksamhet</t>
+  </si>
+  <si>
+    <t>SubjectMail</t>
+  </si>
+  <si>
+    <t>Information saknas i ärendet [CaseID] - Grundskola</t>
   </si>
 </sst>
 </file>
@@ -667,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -855,7 +864,14 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3007,8 +3023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3160,7 +3176,12 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
feat: updating a new function that checks if the type of ride is updated for all the cases that exists in the file. Also added a asset to set how far back from latest run the process should get cases.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Information saknas i ärendet [CaseID] - Grundskola</t>
+  </si>
+  <si>
+    <t>HowFarBackWhenGettingCases</t>
   </si>
 </sst>
 </file>
@@ -676,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -3023,8 +3026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3183,7 +3186,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>

</xml_diff>